<commit_message>
Add data to file
</commit_message>
<xml_diff>
--- a/Homework01/Data/Data.xlsx
+++ b/Homework01/Data/Data.xlsx
@@ -8,18 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josemiguelquinteroholguin/Dropbox/UChicago/2nd Year Classes/Applied-Macro/Homework01/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AEE23C-40D4-F644-877C-D1D3D203F303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404E4CD8-ABE0-D54A-B398-E19369CE5FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{321458A8-742B-DE45-9BC8-5620EF2DE43C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{321458A8-742B-DE45-9BC8-5620EF2DE43C}"/>
   </bookViews>
   <sheets>
     <sheet name="Aggregate" sheetId="1" r:id="rId1"/>
     <sheet name="IPC" sheetId="3" r:id="rId2"/>
     <sheet name="Informality" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Informality!$G$2:$H$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IPC!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet1!$A$2:$B$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet2!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="55">
   <si>
     <t>Ciudad</t>
   </si>
@@ -140,24 +144,86 @@
     <t>Price Index</t>
   </si>
   <si>
-    <t>Informalitty Rate (2018)</t>
-  </si>
-  <si>
-    <t>Informalitty Rate (2015)</t>
-  </si>
-  <si>
     <t>Inf growth</t>
+  </si>
+  <si>
+    <t>Bogotá D.C.</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
+    <t>informality18</t>
+  </si>
+  <si>
+    <t>informality15</t>
+  </si>
+  <si>
+    <t>informality19</t>
+  </si>
+  <si>
+    <t>Cúcuta AM</t>
+  </si>
+  <si>
+    <t>Monteria</t>
+  </si>
+  <si>
+    <t>Santa marta</t>
+  </si>
+  <si>
+    <t>Quibdo</t>
+  </si>
+  <si>
+    <t>Bucaramanga AM</t>
+  </si>
+  <si>
+    <t>Barranquilla AM</t>
+  </si>
+  <si>
+    <t>Popáyan</t>
+  </si>
+  <si>
+    <t>Pereira AM</t>
+  </si>
+  <si>
+    <t>Cali AM</t>
+  </si>
+  <si>
+    <t>Manizales AM</t>
+  </si>
+  <si>
+    <t>Medellin AM</t>
+  </si>
+  <si>
+    <t>informality16</t>
+  </si>
+  <si>
+    <t>Medellin A.M.</t>
+  </si>
+  <si>
+    <t>Popayan</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Growth1518</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,6 +251,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -204,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -236,12 +320,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -257,8 +360,18 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="5" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -574,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C0FD91-A4B1-C94E-8B24-A3805822F578}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,7 +716,7 @@
         <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -622,8 +735,8 @@
       <c r="E2" s="3">
         <v>97.6</v>
       </c>
-      <c r="F2" s="5">
-        <v>-5.9701492537313272E-2</v>
+      <c r="F2" s="8">
+        <v>-1.7999999999999905E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -642,8 +755,8 @@
       <c r="E3" s="3">
         <v>97.26</v>
       </c>
-      <c r="F3" s="5">
-        <v>0</v>
+      <c r="F3" s="8">
+        <v>-3.0000000000001137E-3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -662,8 +775,8 @@
       <c r="E4" s="3">
         <v>97.62</v>
       </c>
-      <c r="F4" s="5">
-        <v>-4.9661399548532548E-2</v>
+      <c r="F4" s="8">
+        <v>-2.5999999999999968E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -682,8 +795,8 @@
       <c r="E5" s="3">
         <v>98.18</v>
       </c>
-      <c r="F5" s="5">
-        <v>3.4734917733089565E-2</v>
+      <c r="F5" s="8">
+        <v>-8.0000000000000071E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -702,8 +815,8 @@
       <c r="E6" s="3">
         <v>97.49</v>
       </c>
-      <c r="F6" s="5">
-        <v>-2.5369978858350906E-2</v>
+      <c r="F6" s="8">
+        <v>-3.4999999999999976E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -722,8 +835,8 @@
       <c r="E7" s="3">
         <v>97.36</v>
       </c>
-      <c r="F7" s="5">
-        <v>5.5045871559631365E-3</v>
+      <c r="F7" s="8">
+        <v>-5.799999999999994E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -742,8 +855,8 @@
       <c r="E8" s="3">
         <v>97.57</v>
       </c>
-      <c r="F8" s="5">
-        <v>2.356406480117812E-2</v>
+      <c r="F8" s="8">
+        <v>-6.9999999999998952E-3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -762,8 +875,8 @@
       <c r="E9" s="3">
         <v>98.07</v>
       </c>
-      <c r="F9" s="5">
-        <v>3.2733224222585955E-2</v>
+      <c r="F9" s="8">
+        <v>-4.7999999999999932E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -782,8 +895,8 @@
       <c r="E10" s="3">
         <v>97.93</v>
       </c>
-      <c r="F10" s="5">
-        <v>-4.3630017452007008E-2</v>
+      <c r="F10" s="8">
+        <v>-6.5999999999999948E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -802,8 +915,8 @@
       <c r="E11" s="3">
         <v>97.69</v>
       </c>
-      <c r="F11" s="5">
-        <v>-2.0979020979021046E-2</v>
+      <c r="F11" s="8">
+        <v>-3.0000000000000027E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -822,8 +935,8 @@
       <c r="E12" s="3">
         <v>97.05</v>
       </c>
-      <c r="F12" s="5">
-        <v>-3.0232558139534738E-2</v>
+      <c r="F12" s="8">
+        <v>2.899999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -842,8 +955,8 @@
       <c r="E13" s="3">
         <v>97.32</v>
       </c>
-      <c r="F13" s="5">
-        <v>9.8360655737705915E-3</v>
+      <c r="F13" s="8">
+        <v>-5.8000000000000052E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -862,8 +975,8 @@
       <c r="E14" s="3">
         <v>97.93</v>
       </c>
-      <c r="F14" s="5">
-        <v>-3.4482758620689724E-3</v>
+      <c r="F14" s="8">
+        <v>-2.0999999999999908E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -882,8 +995,8 @@
       <c r="E15" s="3">
         <v>97.36</v>
       </c>
-      <c r="F15" s="5">
-        <v>-1.5075376884422176E-2</v>
+      <c r="F15" s="8">
+        <v>-4.4999999999999929E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -902,8 +1015,8 @@
       <c r="E16" s="3">
         <v>97.74</v>
       </c>
-      <c r="F16" s="5">
-        <v>2.9182879377432025E-2</v>
+      <c r="F16" s="8">
+        <v>-2.6999999999999968E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -922,8 +1035,8 @@
       <c r="E17" s="3">
         <v>97.57</v>
       </c>
-      <c r="F17" s="5">
-        <v>-6.5630397236614679E-2</v>
+      <c r="F17" s="8">
+        <v>5.1999999999999935E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -942,8 +1055,8 @@
       <c r="E18" s="3">
         <v>97.63</v>
       </c>
-      <c r="F18" s="5">
-        <v>3.2000000000000028E-2</v>
+      <c r="F18" s="8">
+        <v>-8.0000000000000071E-3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -962,8 +1075,8 @@
       <c r="E19" s="3">
         <v>97.83</v>
       </c>
-      <c r="F19" s="5">
-        <v>-2.1739130434782594E-2</v>
+      <c r="F19" s="8">
+        <v>2.7999999999999914E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -982,8 +1095,8 @@
       <c r="E20" s="3">
         <v>97.17</v>
       </c>
-      <c r="F20" s="5">
-        <v>-4.0185471406491535E-2</v>
+      <c r="F20" s="8">
+        <v>-1.100000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1002,8 +1115,8 @@
       <c r="E21" s="3">
         <v>97.16</v>
       </c>
-      <c r="F21" s="5">
-        <v>-3.5123966942148699E-2</v>
+      <c r="F21" s="8">
+        <v>2.899999999999997E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1022,8 +1135,8 @@
       <c r="E22" s="3">
         <v>97.94</v>
       </c>
-      <c r="F22" s="5">
-        <v>-1.0084033613445342E-2</v>
+      <c r="F22" s="8">
+        <v>-3.3000000000000029E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1042,8 +1155,8 @@
       <c r="E23" s="3">
         <v>98.07</v>
       </c>
-      <c r="F23" s="5">
-        <v>-3.3101045296167086E-2</v>
+      <c r="F23" s="8">
+        <v>1.5000000000000013E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1420,29 +1533,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF43465-1DE3-B84B-BBD9-0F1DCC657D16}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1453,11 +1576,19 @@
         <v>0.60299999999999998</v>
       </c>
       <c r="D2">
-        <f>B2/C2-1</f>
-        <v>-5.9701492537313272E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="F2">
+        <v>-5.4123044399317699E-2</v>
+      </c>
+      <c r="H2">
+        <v>-5.4123044399317699E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1468,11 +1599,19 @@
         <v>0.55799999999999994</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D24" si="0">B3/C3-1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.54799999999999993</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="F3">
+        <v>3.7220383980811178E-2</v>
+      </c>
+      <c r="H3">
+        <v>3.7220383980811178E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1483,11 +1622,19 @@
         <v>0.44299999999999995</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>-4.9661399548532548E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.39</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="F4">
+        <v>-8.6126502525891824E-2</v>
+      </c>
+      <c r="H4">
+        <v>-8.6126502525891824E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1498,11 +1645,19 @@
         <v>0.54700000000000004</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>3.4734917733089565E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="F5">
+        <v>5.5660624724542584E-2</v>
+      </c>
+      <c r="H5">
+        <v>5.5660624724542584E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1513,11 +1668,19 @@
         <v>0.47299999999999998</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>-2.5369978858350906E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.49</v>
+      </c>
+      <c r="F6">
+        <v>5.6284816010971905E-3</v>
+      </c>
+      <c r="H6">
+        <v>5.6284816010971905E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1528,11 +1691,19 @@
         <v>0.54500000000000004</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>5.5045871559631365E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="F7">
+        <v>1.6293351476585283E-2</v>
+      </c>
+      <c r="H7">
+        <v>1.6293351476585283E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1543,11 +1714,19 @@
         <v>0.67900000000000005</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>2.356406480117812E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.69400000000000006</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="F8">
+        <v>-5.9086800273385753E-3</v>
+      </c>
+      <c r="H8">
+        <v>-5.9086800273385753E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1558,11 +1737,19 @@
         <v>0.61099999999999999</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>3.2733224222585955E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.58700000000000008</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="F9">
+        <v>5.995632145288643E-2</v>
+      </c>
+      <c r="H9">
+        <v>5.995632145288643E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1573,11 +1760,19 @@
         <v>0.57299999999999995</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>-4.3630017452007008E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="F10">
+        <v>-2.3034263255612197E-2</v>
+      </c>
+      <c r="H10">
+        <v>-2.3034263255612197E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1588,11 +1783,19 @@
         <v>0.42899999999999999</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>-2.0979020979021046E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.438</v>
+      </c>
+      <c r="F11">
+        <v>-3.2437764516155432E-2</v>
+      </c>
+      <c r="H11">
+        <v>-3.2437764516155432E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1603,11 +1806,19 @@
         <v>0.43</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>-3.0232558139534738E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.433</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="F12">
+        <v>1.2580913536641702E-4</v>
+      </c>
+      <c r="H12">
+        <v>1.2580913536641702E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1618,11 +1829,19 @@
         <v>0.61</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>9.8360655737705915E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="F13">
+        <v>2.620325658190148E-2</v>
+      </c>
+      <c r="H13">
+        <v>2.620325658190148E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1633,11 +1852,19 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>-3.4482758620689724E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="F14">
+        <v>1.324221890432975E-2</v>
+      </c>
+      <c r="H14">
+        <v>1.324221890432975E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1648,11 +1875,19 @@
         <v>0.59699999999999998</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>-1.5075376884422176E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="F15">
+        <v>7.1473185001051487E-2</v>
+      </c>
+      <c r="H15">
+        <v>7.1473185001051487E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1663,11 +1898,19 @@
         <v>0.51400000000000001</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>2.9182879377432025E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.49200000000000005</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="F16">
+        <v>0.10924796283255445</v>
+      </c>
+      <c r="H16">
+        <v>0.10924796283255445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1678,11 +1921,19 @@
         <v>0.57899999999999996</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>-6.5630397236614679E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="F17">
+        <v>-6.6440447541099568E-3</v>
+      </c>
+      <c r="H17">
+        <v>-6.6440447541099568E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1693,11 +1944,19 @@
         <v>0.63200000000000001</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>-0.10759493670886089</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="F18">
+        <v>-0.18539947374715959</v>
+      </c>
+      <c r="H18">
+        <v>0.1323309598440936</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1708,11 +1967,19 @@
         <v>0.625</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>3.2000000000000028E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="F19">
+        <v>0.1323309598440936</v>
+      </c>
+      <c r="H19">
+        <v>2.4241494177755118E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1723,11 +1990,19 @@
         <v>0.64400000000000002</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>-2.1739130434782594E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.6409999999999999</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="F20">
+        <v>2.4241494177755118E-2</v>
+      </c>
+      <c r="H20">
+        <v>7.5842482035887837E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1738,11 +2013,19 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
-        <v>-4.0185471406491535E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="F21">
+        <v>7.5842482035887837E-2</v>
+      </c>
+      <c r="H21">
+        <v>-2.372881355932166E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1753,11 +2036,19 @@
         <v>0.48399999999999999</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
-        <v>-3.5123966942148699E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.49</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="F22">
+        <v>-2.372881355932166E-3</v>
+      </c>
+      <c r="H22">
+        <v>2.8491259893290488E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1768,11 +2059,19 @@
         <v>0.59499999999999997</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
-        <v>-1.0084033613445342E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0.624</v>
+      </c>
+      <c r="F23">
+        <v>2.8491259893290488E-2</v>
+      </c>
+      <c r="H23">
+        <v>3.3107014005284041E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1783,11 +2082,474 @@
         <v>0.57399999999999995</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
-        <v>-3.3101045296167086E-2</v>
+        <v>0.57100000000000006</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="F24">
+        <v>3.3107014005284041E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC024774-E462-3340-9C3A-7CE1158C6CE8}">
+  <dimension ref="A2:XFD25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="XFD2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.1323309598440936</v>
+      </c>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>3.7220383980811178E-2</v>
+      </c>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>-8.6126502525891824E-2</v>
+      </c>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>5.5660624724542584E-2</v>
+      </c>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>5.6284816010971905E-3</v>
+      </c>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2.620325658190148E-2</v>
+      </c>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>0.10924796283255445</v>
+      </c>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>-2.372881355932166E-3</v>
+      </c>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>-5.9086800273385753E-3</v>
+      </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <v>1.2580913536641702E-4</v>
+      </c>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>-2.3034263255612197E-2</v>
+      </c>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>2.8491259893290488E-2</v>
+      </c>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>-3.2437764516155432E-2</v>
+      </c>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>7.1473185001051487E-2</v>
+      </c>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18">
+        <v>5.995632145288643E-2</v>
+      </c>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>-0.18539947374715959</v>
+      </c>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21">
+        <v>1.324221890432975E-2</v>
+      </c>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>3.3107014005284041E-2</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="I23">
+        <v>2.4241494177755118E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>-6.6440447541099568E-3</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="I24">
+        <v>-5.4123044399317699E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>1.6293351476585283E-2</v>
+      </c>
+      <c r="I25">
+        <v>7.5842482035887837E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:B2" xr:uid="{EC024774-E462-3340-9C3A-7CE1158C6CE8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B25">
+      <sortCondition ref="A2:A25"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F421C15-E356-DC49-B437-372CC71C4FFC}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-5.4123044399317699E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3.7220383980811178E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-8.6126502525891824E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>5.5660624724542584E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5.6284816010971905E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1.6293351476585283E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-5.9086800273385753E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5.995632145288643E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-2.3034263255612197E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-3.2437764516155432E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>1.2580913536641702E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>2.620325658190148E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1.324221890432975E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>7.1473185001051487E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.10924796283255445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>-6.6440447541099568E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18">
+        <v>-0.18539947374715959</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0.1323309598440936</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>2.4241494177755118E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>7.5842482035887837E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>-2.372881355932166E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2.8491259893290488E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>3.3107014005284041E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{2F421C15-E356-DC49-B437-372CC71C4FFC}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B24">
+      <sortCondition ref="A1:A24"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>